<commit_message>
2; 24; 7; 15
</commit_message>
<xml_diff>
--- a/Книга2.xlsx
+++ b/Книга2.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stepan_\Documents\Informatica\Informatica_EGE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CB6D9B9-491D-4CCA-BEF6-8DCEA260C1D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EFA4AFD-90DC-4700-B1C7-9420A76F3EA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15675" xr2:uid="{5D558663-B315-457E-85D7-119A94F0FD92}"/>
   </bookViews>
@@ -465,7 +465,7 @@
   <dimension ref="A1:AA16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="P7" sqref="P7"/>
+      <selection activeCell="R17" sqref="R17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.3984375" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -846,41 +846,63 @@
     </row>
     <row r="8" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A8" s="3">
-        <v>45649</v>
-      </c>
-      <c r="B8" s="1"/>
+        <v>45670</v>
+      </c>
+      <c r="B8" s="1">
+        <v>5</v>
+      </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
+      <c r="E8" s="1">
+        <v>5</v>
+      </c>
+      <c r="F8" s="1">
+        <v>5</v>
+      </c>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
-      <c r="J8" s="1"/>
-      <c r="K8" s="1"/>
+      <c r="J8" s="1">
+        <v>5</v>
+      </c>
+      <c r="K8" s="1">
+        <v>5</v>
+      </c>
       <c r="L8" s="1"/>
       <c r="M8" s="1"/>
-      <c r="N8" s="1"/>
+      <c r="N8" s="1">
+        <v>5</v>
+      </c>
       <c r="O8" s="1"/>
       <c r="P8" s="1"/>
       <c r="Q8" s="1"/>
-      <c r="R8" s="1"/>
+      <c r="R8" s="1">
+        <v>5</v>
+      </c>
       <c r="S8" s="1"/>
-      <c r="T8" s="1"/>
+      <c r="T8" s="1">
+        <v>5</v>
+      </c>
       <c r="U8" s="1"/>
       <c r="V8" s="1"/>
       <c r="W8" s="1"/>
-      <c r="X8" s="1"/>
-      <c r="Y8" s="1"/>
-      <c r="Z8" s="1"/>
+      <c r="X8" s="1">
+        <v>5</v>
+      </c>
+      <c r="Y8" s="1">
+        <v>5</v>
+      </c>
+      <c r="Z8" s="1">
+        <v>5</v>
+      </c>
       <c r="AA8" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>55</v>
       </c>
     </row>
     <row r="9" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A9" s="3">
-        <v>45656</v>
+        <v>45677</v>
       </c>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -914,7 +936,7 @@
     </row>
     <row r="10" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A10" s="3">
-        <v>45663</v>
+        <v>45684</v>
       </c>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -948,7 +970,7 @@
     </row>
     <row r="11" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A11" s="3">
-        <v>45670</v>
+        <v>45691</v>
       </c>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -982,7 +1004,7 @@
     </row>
     <row r="12" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A12" s="3">
-        <v>45677</v>
+        <v>45698</v>
       </c>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -1016,7 +1038,7 @@
     </row>
     <row r="13" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A13" s="3">
-        <v>45684</v>
+        <v>45705</v>
       </c>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -1050,7 +1072,7 @@
     </row>
     <row r="14" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A14" s="3">
-        <v>45691</v>
+        <v>45712</v>
       </c>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -1084,7 +1106,7 @@
     </row>
     <row r="15" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A15" s="3">
-        <v>45698</v>
+        <v>45719</v>
       </c>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -1122,7 +1144,7 @@
       </c>
       <c r="B16" s="2">
         <f>SUM(B2:B15)</f>
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C16" s="2">
         <f t="shared" ref="C16:AA16" si="1">SUM(C2:C15)</f>
@@ -1134,11 +1156,11 @@
       </c>
       <c r="E16" s="2">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="F16" s="2">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="G16" s="2">
         <f t="shared" si="1"/>
@@ -1154,11 +1176,11 @@
       </c>
       <c r="J16" s="2">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="K16" s="2">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="L16" s="2">
         <f t="shared" si="1"/>
@@ -1170,59 +1192,59 @@
       </c>
       <c r="N16" s="2">
         <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="O16" s="2">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="P16" s="2">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="Q16" s="2">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="R16" s="2">
+        <f t="shared" si="1"/>
         <v>15</v>
       </c>
-      <c r="O16" s="2">
-        <f t="shared" si="1"/>
-        <v>10</v>
-      </c>
-      <c r="P16" s="2">
-        <f t="shared" si="1"/>
-        <v>10</v>
-      </c>
-      <c r="Q16" s="2">
-        <f t="shared" si="1"/>
-        <v>10</v>
-      </c>
-      <c r="R16" s="2">
-        <f t="shared" si="1"/>
-        <v>10</v>
-      </c>
       <c r="S16" s="2">
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="T16" s="2">
         <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="U16" s="2">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="V16" s="2">
+        <f t="shared" si="1"/>
         <v>15</v>
       </c>
-      <c r="U16" s="2">
-        <f t="shared" si="1"/>
-        <v>10</v>
-      </c>
-      <c r="V16" s="2">
+      <c r="W16" s="2">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="X16" s="2">
         <f t="shared" si="1"/>
         <v>15</v>
       </c>
-      <c r="W16" s="2">
-        <f t="shared" si="1"/>
-        <v>10</v>
-      </c>
-      <c r="X16" s="2">
-        <f t="shared" si="1"/>
-        <v>10</v>
-      </c>
       <c r="Y16" s="2">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="Z16" s="2">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AA16" s="2">
         <f t="shared" si="1"/>
-        <v>230</v>
+        <v>285</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
11; 12; 14; 15; 16; 19-21; 25; 26; 27; 6; 7; 8
</commit_message>
<xml_diff>
--- a/Книга2.xlsx
+++ b/Книга2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stepan_\Documents\Informatica\Informatica_EGE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EFA4AFD-90DC-4700-B1C7-9420A76F3EA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F32B0682-6E7A-4DE3-B433-ABB05EECEA34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15675" xr2:uid="{5D558663-B315-457E-85D7-119A94F0FD92}"/>
   </bookViews>
@@ -465,7 +465,7 @@
   <dimension ref="A1:AA16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="R17" sqref="R17"/>
+      <selection activeCell="O9" sqref="O9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.3984375" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -902,24 +902,40 @@
     </row>
     <row r="9" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A9" s="3">
-        <v>45677</v>
+        <v>45684</v>
       </c>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
+      <c r="G9" s="1">
+        <v>5</v>
+      </c>
+      <c r="H9" s="1">
+        <v>5</v>
+      </c>
+      <c r="I9" s="1">
+        <v>5</v>
+      </c>
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
-      <c r="L9" s="1"/>
-      <c r="M9" s="1"/>
+      <c r="L9" s="1">
+        <v>5</v>
+      </c>
+      <c r="M9" s="1">
+        <v>5</v>
+      </c>
       <c r="N9" s="1"/>
-      <c r="O9" s="1"/>
-      <c r="P9" s="1"/>
-      <c r="Q9" s="1"/>
+      <c r="O9" s="1">
+        <v>5</v>
+      </c>
+      <c r="P9" s="1">
+        <v>5</v>
+      </c>
+      <c r="Q9" s="1">
+        <v>5</v>
+      </c>
       <c r="R9" s="1"/>
       <c r="S9" s="1"/>
       <c r="T9" s="1"/>
@@ -931,12 +947,12 @@
       <c r="Z9" s="1"/>
       <c r="AA9" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A10" s="3">
-        <v>45684</v>
+        <v>45691</v>
       </c>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -970,7 +986,7 @@
     </row>
     <row r="11" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A11" s="3">
-        <v>45691</v>
+        <v>45698</v>
       </c>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -1004,7 +1020,7 @@
     </row>
     <row r="12" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A12" s="3">
-        <v>45698</v>
+        <v>45705</v>
       </c>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -1038,7 +1054,7 @@
     </row>
     <row r="13" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A13" s="3">
-        <v>45705</v>
+        <v>45712</v>
       </c>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -1072,7 +1088,7 @@
     </row>
     <row r="14" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A14" s="3">
-        <v>45712</v>
+        <v>45719</v>
       </c>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -1106,7 +1122,7 @@
     </row>
     <row r="15" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A15" s="3">
-        <v>45719</v>
+        <v>45726</v>
       </c>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -1164,15 +1180,15 @@
       </c>
       <c r="G16" s="2">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="H16" s="2">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="I16" s="2">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="J16" s="2">
         <f t="shared" si="1"/>
@@ -1184,11 +1200,11 @@
       </c>
       <c r="L16" s="2">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="M16" s="2">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="N16" s="2">
         <f t="shared" si="1"/>
@@ -1196,15 +1212,15 @@
       </c>
       <c r="O16" s="2">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="P16" s="2">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="Q16" s="2">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="R16" s="2">
         <f t="shared" si="1"/>
@@ -1244,7 +1260,7 @@
       </c>
       <c r="AA16" s="2">
         <f t="shared" si="1"/>
-        <v>285</v>
+        <v>325</v>
       </c>
     </row>
   </sheetData>

</xml_diff>